<commit_message>
porównanie wyników klasyfikacji (RF, SVM, NN, NB) i klasteryzacji (K-means) z publikacją
</commit_message>
<xml_diff>
--- a/porównanie wyników.xlsx
+++ b/porównanie wyników.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\Documents\wyniki\1607\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3959D3AD-F24D-47A9-A1CA-E942A69FCB27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E72B9E-29A3-4139-A4AF-32DF6235DE77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="41">
   <si>
     <t>Klasyfikacja:</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Kmeans wytrenowane na pliku .csv z publikacji na github (próbki i cechy z publikacji):</t>
+  </si>
+  <si>
+    <t>PCA z pliku .csv z publikacji na github (próbki i cechy z publikacji):</t>
+  </si>
+  <si>
+    <t>PCA z pliku powstałego po dodaniu nowych cech (moje próbki, moje cechy):</t>
+  </si>
+  <si>
+    <t>PCA tylko z cechami z publikacji (moje próbki, cechy z publikacji):</t>
   </si>
 </sst>
 </file>
@@ -713,6 +722,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>205226</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>14897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BE50DF4-3829-4A73-A295-0F5047E6FC1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9502140" y="563880"/>
+          <a:ext cx="4114286" cy="2742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>456686</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>182537</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Obraz 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{926A1DF4-26CC-4D7E-8768-D0E33E91BBE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="548640"/>
+          <a:ext cx="4114286" cy="2742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>319526</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>159677</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Obraz 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{024A0F1D-9F59-40F9-91A0-1F217391C920}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4739640" y="525780"/>
+          <a:ext cx="4114286" cy="2742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1012,1088 +1158,519 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R74"/>
+  <dimension ref="A2:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="62" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P4" s="3" t="s">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I25" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P25" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I26" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P26" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I27" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P27" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A10" s="1" t="s">
+    <row r="30" spans="1:16" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" t="s">
-        <v>13</v>
-      </c>
-      <c r="P13" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>12</v>
-      </c>
-      <c r="R13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>15</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>5</v>
-      </c>
-      <c r="P14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="I15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-      <c r="K15">
-        <v>18</v>
-      </c>
-      <c r="P15" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>82</v>
-      </c>
-      <c r="I16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="K16">
-        <v>79</v>
-      </c>
-      <c r="P16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q16">
-        <v>2</v>
-      </c>
-      <c r="R16">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="I17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17">
-        <v>4</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="P17" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q17">
-        <v>3</v>
-      </c>
-      <c r="R17">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18">
-        <v>10</v>
-      </c>
-      <c r="K18">
-        <v>2</v>
-      </c>
-      <c r="P18" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q18">
-        <v>6</v>
-      </c>
-      <c r="R18">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>28</v>
-      </c>
-      <c r="I19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>19</v>
-      </c>
-      <c r="P19" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q19">
-        <v>8</v>
-      </c>
-      <c r="R19">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <v>5</v>
-      </c>
-      <c r="P20" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q20">
-        <v>9</v>
-      </c>
-      <c r="R20">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>76</v>
-      </c>
-      <c r="I21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-      <c r="K21">
-        <v>13</v>
-      </c>
-      <c r="P21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q21">
-        <v>10</v>
-      </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="I22" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22">
-        <v>4</v>
-      </c>
-      <c r="K22">
-        <v>28</v>
-      </c>
-      <c r="P22" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23">
-        <v>7</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23">
-        <v>5</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>40</v>
-      </c>
-      <c r="I24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24">
-        <v>6</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="P24" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q24">
-        <v>2</v>
-      </c>
-      <c r="R24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25">
-        <v>10</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="I25" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25">
-        <v>8</v>
-      </c>
-      <c r="K25">
-        <v>78</v>
-      </c>
-      <c r="P25" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q25">
-        <v>5</v>
-      </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>55</v>
-      </c>
-      <c r="I26" t="s">
-        <v>15</v>
-      </c>
-      <c r="J26">
-        <v>9</v>
-      </c>
-      <c r="K26">
-        <v>3</v>
-      </c>
-      <c r="P26" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q26">
-        <v>6</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>86</v>
-      </c>
-      <c r="I27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27">
-        <v>10</v>
-      </c>
-      <c r="K27">
-        <v>2</v>
-      </c>
-      <c r="P27" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q27">
-        <v>8</v>
-      </c>
-      <c r="R27">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>136</v>
-      </c>
-      <c r="I28" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>54</v>
-      </c>
-      <c r="P28" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q28">
-        <v>9</v>
-      </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29">
-        <v>7</v>
-      </c>
-      <c r="C29">
-        <v>8</v>
-      </c>
-      <c r="I29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29">
-        <v>7</v>
-      </c>
-      <c r="K29">
-        <v>87</v>
-      </c>
-      <c r="P29" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q29">
-        <v>10</v>
-      </c>
-      <c r="R29">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30">
-        <v>8</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="I30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30">
-        <v>2</v>
-      </c>
-      <c r="K30">
-        <v>126</v>
-      </c>
-      <c r="P30" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31">
-        <v>10</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="I31" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31">
-        <v>3</v>
-      </c>
-      <c r="K31">
-        <v>21</v>
-      </c>
-      <c r="P31" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q31">
-        <v>1</v>
-      </c>
-      <c r="R31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>62</v>
-      </c>
-      <c r="I32" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32">
-        <v>9</v>
-      </c>
-      <c r="K32">
-        <v>3</v>
-      </c>
-      <c r="P32" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q32">
-        <v>2</v>
-      </c>
-      <c r="R32">
-        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
       </c>
       <c r="I33" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>65</v>
+        <v>11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" t="s">
+        <v>13</v>
       </c>
       <c r="P33" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q33">
-        <v>3</v>
-      </c>
-      <c r="R33">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>12</v>
+      </c>
+      <c r="R33" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I34" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K34">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P34" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q34">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B35">
         <v>6</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35">
         <v>18</v>
       </c>
-      <c r="J35">
-        <v>3</v>
-      </c>
-      <c r="K35">
-        <v>9</v>
-      </c>
       <c r="P35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q35">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="R35">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B36">
         <v>7</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="I36" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K36">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="P36" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q36">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="R36">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B37">
         <v>8</v>
       </c>
       <c r="C37">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K37">
         <v>1</v>
       </c>
       <c r="P37" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q37">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R37">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J38">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K38">
         <v>2</v>
       </c>
       <c r="P38" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="Q38">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R38">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>28</v>
+      </c>
+      <c r="I39" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
         <v>19</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="I39" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39">
-        <v>10</v>
-      </c>
-      <c r="K39">
-        <v>13</v>
-      </c>
       <c r="P39" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="Q39">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R39">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
         <v>5</v>
       </c>
-      <c r="I40" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
-        <v>3</v>
-      </c>
       <c r="P40" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="Q40">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R40">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="I41" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K41">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="P41" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="Q41">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R41">
-        <v>111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42">
         <v>4</v>
       </c>
-      <c r="I42" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42">
-        <v>3</v>
-      </c>
       <c r="K42">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="P42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q42">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R42">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="P43" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
         <v>8</v>
-      </c>
-      <c r="C43">
-        <v>17</v>
-      </c>
-      <c r="I43" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43">
-        <v>4</v>
-      </c>
-      <c r="K43">
-        <v>15</v>
-      </c>
-      <c r="P43" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q43">
-        <v>4</v>
-      </c>
-      <c r="R43">
-        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I44" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K44">
         <v>1</v>
       </c>
       <c r="P44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J45">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K45">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="P45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R45">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C46">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="I46" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J46">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K46">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P46" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q46">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R46">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="I47" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J47">
         <v>10</v>
@@ -2102,126 +1679,126 @@
         <v>2</v>
       </c>
       <c r="P47" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q47">
         <v>8</v>
       </c>
       <c r="R47">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="I48" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="P48" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q48">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R48">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I49" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K49">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="P49" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="Q49">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R49">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K50">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="P50" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="Q50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R50">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="I51" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
         <v>21</v>
       </c>
-      <c r="B51">
-        <v>6</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="I51" t="s">
-        <v>20</v>
-      </c>
-      <c r="J51">
-        <v>7</v>
-      </c>
-      <c r="K51">
-        <v>1</v>
-      </c>
       <c r="P51" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="Q51">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R51">
         <v>1</v>
@@ -2229,260 +1806,260 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C52">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="I52" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J52">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K52">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P52" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="Q52">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="R52">
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J53">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K53">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="P53" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="Q53">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="R53">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B54">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J54">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K54">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="P54" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="Q54">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R54">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="I55" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K55">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P55" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="Q55">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R55">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C56">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I56" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J56">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P56" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="Q56">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R56">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C57">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="I57" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J57">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K57">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="P57" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="Q57">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R57">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I58" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J58">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P58" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="Q58">
         <v>2</v>
       </c>
       <c r="R58">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B59">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J59">
         <v>10</v>
       </c>
       <c r="K59">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="P59" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="Q59">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R59">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C60">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I60" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J60">
         <v>1</v>
       </c>
       <c r="K60">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="P60" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="Q60">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="R60">
         <v>2</v>
@@ -2490,304 +2067,885 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I61" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J61">
         <v>2</v>
       </c>
       <c r="K61">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P61" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="Q61">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="R61">
-        <v>171</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C62">
-        <v>143</v>
+        <v>4</v>
       </c>
       <c r="I62" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J62">
         <v>3</v>
       </c>
       <c r="K62">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="P62" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="Q62">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="R62">
-        <v>68</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I63" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J63">
         <v>4</v>
       </c>
       <c r="K63">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="P63" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="Q63">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="R63">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="J64">
+        <v>5</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="P64" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q64">
+        <v>5</v>
+      </c>
+      <c r="R64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="I65" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65">
+        <v>6</v>
+      </c>
+      <c r="K65">
+        <v>2</v>
+      </c>
+      <c r="P65" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q65">
+        <v>6</v>
+      </c>
+      <c r="R65">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
+      </c>
+      <c r="C66">
+        <v>11</v>
+      </c>
+      <c r="I66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66">
+        <v>8</v>
+      </c>
+      <c r="K66">
+        <v>5</v>
+      </c>
+      <c r="P66" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q66">
+        <v>7</v>
+      </c>
+      <c r="R66">
         <v>9</v>
       </c>
-      <c r="C64">
-        <v>150</v>
-      </c>
-      <c r="I64" t="s">
-        <v>22</v>
-      </c>
-      <c r="J64">
-        <v>6</v>
-      </c>
-      <c r="K64">
-        <v>3</v>
-      </c>
-      <c r="P64" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q64">
-        <v>10</v>
-      </c>
-      <c r="R64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I65" t="s">
-        <v>22</v>
-      </c>
-      <c r="J65">
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67">
         <v>8</v>
       </c>
-      <c r="K65">
-        <v>1</v>
-      </c>
-      <c r="P65" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q65">
-        <v>1</v>
-      </c>
-      <c r="R65">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I66" t="s">
-        <v>22</v>
-      </c>
-      <c r="J66">
+      <c r="C67">
         <v>9</v>
       </c>
-      <c r="K66">
-        <v>6</v>
-      </c>
-      <c r="P66" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q66">
-        <v>5</v>
-      </c>
-      <c r="R66">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I67" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J67">
         <v>10</v>
       </c>
       <c r="K67">
+        <v>2</v>
+      </c>
+      <c r="P67" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q67">
+        <v>8</v>
+      </c>
+      <c r="R67">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>123</v>
+      </c>
+      <c r="I68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J68">
+        <v>2</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="P68" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69">
+        <v>3</v>
+      </c>
+      <c r="K69">
+        <v>11</v>
+      </c>
+      <c r="P69" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q69">
+        <v>1</v>
+      </c>
+      <c r="R69">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
+      </c>
+      <c r="J70">
+        <v>4</v>
+      </c>
+      <c r="K70">
+        <v>6</v>
+      </c>
+      <c r="P70" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q70">
+        <v>2</v>
+      </c>
+      <c r="R70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="I71" t="s">
+        <v>20</v>
+      </c>
+      <c r="J71">
         <v>7</v>
       </c>
-      <c r="P67" t="s">
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="P71" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q71">
+        <v>5</v>
+      </c>
+      <c r="R71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>7</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
+      </c>
+      <c r="J72">
+        <v>8</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="P72" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q72">
+        <v>6</v>
+      </c>
+      <c r="R72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73">
+        <v>8</v>
+      </c>
+      <c r="C73">
+        <v>12</v>
+      </c>
+      <c r="I73" t="s">
+        <v>20</v>
+      </c>
+      <c r="J73">
+        <v>9</v>
+      </c>
+      <c r="K73">
+        <v>121</v>
+      </c>
+      <c r="P73" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q73">
+        <v>8</v>
+      </c>
+      <c r="R73">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74">
+        <v>10</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>20</v>
+      </c>
+      <c r="J74">
+        <v>10</v>
+      </c>
+      <c r="K74">
+        <v>9</v>
+      </c>
+      <c r="P74" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q74">
+        <v>9</v>
+      </c>
+      <c r="R74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
         <v>23</v>
       </c>
-      <c r="Q67">
+      <c r="I75" t="s">
+        <v>21</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>2</v>
+      </c>
+      <c r="P75" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q75">
+        <v>10</v>
+      </c>
+      <c r="R75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="I76" t="s">
+        <v>21</v>
+      </c>
+      <c r="J76">
+        <v>2</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="P76" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77">
         <v>6</v>
       </c>
-      <c r="R67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I68" t="s">
+      <c r="C77">
+        <v>52</v>
+      </c>
+      <c r="I77" t="s">
+        <v>21</v>
+      </c>
+      <c r="J77">
+        <v>3</v>
+      </c>
+      <c r="K77">
+        <v>20</v>
+      </c>
+      <c r="P77" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q77">
+        <v>1</v>
+      </c>
+      <c r="R77">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78">
+        <v>16</v>
+      </c>
+      <c r="I78" t="s">
+        <v>21</v>
+      </c>
+      <c r="J78">
+        <v>9</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="P78" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q78">
+        <v>2</v>
+      </c>
+      <c r="R78">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>81</v>
+      </c>
+      <c r="I79" t="s">
+        <v>21</v>
+      </c>
+      <c r="J79">
+        <v>10</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="P79" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q79">
+        <v>3</v>
+      </c>
+      <c r="R79">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>23</v>
       </c>
-      <c r="J68">
-        <v>1</v>
-      </c>
-      <c r="K68">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>4</v>
+      </c>
+      <c r="I80" t="s">
+        <v>22</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>23</v>
+      </c>
+      <c r="P80" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q80">
+        <v>5</v>
+      </c>
+      <c r="R80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="I81" t="s">
+        <v>22</v>
+      </c>
+      <c r="J81">
+        <v>2</v>
+      </c>
+      <c r="K81">
+        <v>5</v>
+      </c>
+      <c r="P81" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q81">
+        <v>6</v>
+      </c>
+      <c r="R81">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <v>143</v>
+      </c>
+      <c r="I82" t="s">
+        <v>22</v>
+      </c>
+      <c r="J82">
+        <v>3</v>
+      </c>
+      <c r="K82">
+        <v>67</v>
+      </c>
+      <c r="P82" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q82">
+        <v>8</v>
+      </c>
+      <c r="R82">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83">
+        <v>7</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="I83" t="s">
+        <v>22</v>
+      </c>
+      <c r="J83">
+        <v>4</v>
+      </c>
+      <c r="K83">
+        <v>63</v>
+      </c>
+      <c r="P83" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q83">
+        <v>9</v>
+      </c>
+      <c r="R83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <v>150</v>
+      </c>
+      <c r="I84" t="s">
+        <v>22</v>
+      </c>
+      <c r="J84">
+        <v>6</v>
+      </c>
+      <c r="K84">
+        <v>3</v>
+      </c>
+      <c r="P84" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q84">
+        <v>10</v>
+      </c>
+      <c r="R84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I85" t="s">
+        <v>22</v>
+      </c>
+      <c r="J85">
+        <v>8</v>
+      </c>
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="P85" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q85">
+        <v>1</v>
+      </c>
+      <c r="R85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I86" t="s">
+        <v>22</v>
+      </c>
+      <c r="J86">
+        <v>9</v>
+      </c>
+      <c r="K86">
+        <v>6</v>
+      </c>
+      <c r="P86" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q86">
+        <v>5</v>
+      </c>
+      <c r="R86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I87" t="s">
+        <v>22</v>
+      </c>
+      <c r="J87">
+        <v>10</v>
+      </c>
+      <c r="K87">
+        <v>7</v>
+      </c>
+      <c r="P87" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q87">
+        <v>6</v>
+      </c>
+      <c r="R87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I88" t="s">
+        <v>23</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88">
         <v>13</v>
       </c>
-      <c r="P68" t="s">
+      <c r="P88" t="s">
         <v>23</v>
       </c>
-      <c r="Q68">
+      <c r="Q88">
         <v>7</v>
       </c>
-      <c r="R68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I69" t="s">
+      <c r="R88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I89" t="s">
         <v>23</v>
       </c>
-      <c r="J69">
-        <v>2</v>
-      </c>
-      <c r="K69">
+      <c r="J89">
+        <v>2</v>
+      </c>
+      <c r="K89">
         <v>4</v>
       </c>
-      <c r="P69" t="s">
+      <c r="P89" t="s">
         <v>23</v>
       </c>
-      <c r="Q69">
+      <c r="Q89">
         <v>8</v>
       </c>
-      <c r="R69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I70" t="s">
+      <c r="R89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I90" t="s">
         <v>23</v>
       </c>
-      <c r="J70">
+      <c r="J90">
         <v>6</v>
       </c>
-      <c r="K70">
+      <c r="K90">
         <v>132</v>
       </c>
-      <c r="P70" t="s">
+      <c r="P90" t="s">
         <v>35</v>
       </c>
-      <c r="Q70">
-        <v>1</v>
-      </c>
-      <c r="R70">
+      <c r="Q90">
+        <v>1</v>
+      </c>
+      <c r="R90">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I71" t="s">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I91" t="s">
         <v>23</v>
       </c>
-      <c r="J71">
+      <c r="J91">
         <v>10</v>
       </c>
-      <c r="K71">
-        <v>1</v>
-      </c>
-      <c r="P71" t="s">
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="P91" t="s">
         <v>35</v>
       </c>
-      <c r="Q71">
+      <c r="Q91">
         <v>8</v>
       </c>
-      <c r="R71">
+      <c r="R91">
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="I72" t="s">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I92" t="s">
         <v>24</v>
       </c>
-      <c r="J72">
+      <c r="J92">
         <v>5</v>
       </c>
-      <c r="K72">
+      <c r="K92">
         <v>150</v>
       </c>
-      <c r="P72" t="s">
+      <c r="P92" t="s">
         <v>35</v>
       </c>
-      <c r="Q72">
+      <c r="Q92">
         <v>9</v>
       </c>
-      <c r="R72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="P73" t="s">
+      <c r="R92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P93" t="s">
         <v>24</v>
       </c>
-      <c r="Q73">
+      <c r="Q93">
         <v>4</v>
       </c>
-      <c r="R73">
+      <c r="R93">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="P74" t="s">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P94" t="s">
         <v>24</v>
       </c>
-      <c r="Q74">
+      <c r="Q94">
         <v>7</v>
       </c>
-      <c r="R74">
+      <c r="R94">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>